<commit_message>
nonproductive-alarm data api completed
</commit_message>
<xml_diff>
--- a/doc/proj/需求/报表开发.xlsx
+++ b/doc/proj/需求/报表开发.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\PueProject\doc\proj\需求\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\ThinkingAgain\PueProject\doc\proj\需求\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E833A05E-0B43-40B2-9259-7A8521BB40CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A71CCC-D007-4DFF-986D-376E2D3043E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="全市用电报表" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
   <si>
     <t>能源系统信息</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>看看哪个口径好统计</t>
-  </si>
-  <si>
-    <t>用电流换算用夜间电量？电流*220/54*1.52/24*小时数</t>
   </si>
   <si>
     <t>电流信息</t>
@@ -194,6 +191,22 @@
   <si>
     <t>时间</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>办公+营业&gt;1A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分成2个: 平均和最大</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用电流换算用夜间电量？电流*220/54*1.52/24*小时数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当日22:00 - 次日 06:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -282,7 +295,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -309,6 +322,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -622,47 +638,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.15625" customWidth="1"/>
-    <col min="2" max="2" width="23.20703125" customWidth="1"/>
-    <col min="3" max="3" width="8.20703125" customWidth="1"/>
-    <col min="6" max="8" width="12.89453125" customWidth="1"/>
-    <col min="9" max="9" width="11.89453125" customWidth="1"/>
-    <col min="10" max="12" width="12.89453125" customWidth="1"/>
-    <col min="13" max="13" width="10.89453125" customWidth="1"/>
+    <col min="1" max="1" width="15.1796875" customWidth="1"/>
+    <col min="2" max="2" width="23.1796875" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" customWidth="1"/>
+    <col min="6" max="8" width="12.90625" customWidth="1"/>
+    <col min="9" max="9" width="11.90625" customWidth="1"/>
+    <col min="10" max="12" width="12.90625" customWidth="1"/>
+    <col min="13" max="13" width="10.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9" t="s">
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
       <c r="O1" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -670,7 +686,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -707,161 +723,161 @@
       </c>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -878,21 +894,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.26171875" customWidth="1"/>
-    <col min="2" max="2" width="22.62890625" customWidth="1"/>
-    <col min="3" max="3" width="21.26171875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="48.89453125" customWidth="1"/>
+    <col min="1" max="1" width="11.26953125" customWidth="1"/>
+    <col min="2" max="2" width="22.6328125" customWidth="1"/>
+    <col min="3" max="3" width="21.26953125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="48.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -906,7 +922,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>22</v>
@@ -914,40 +930,50 @@
       <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D2" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="1"/>
+      <c r="C3" s="9" t="s">
+        <v>52</v>
+      </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="1"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="1"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
+      <c r="D7" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -964,46 +990,46 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.89453125" customWidth="1"/>
-    <col min="7" max="8" width="12.89453125" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" customWidth="1"/>
+    <col min="7" max="8" width="12.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>8</v>
@@ -1018,9 +1044,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>